<commit_message>
Penambahan fitur harga grosir dengan 3 level
</commit_message>
<xml_diff>
--- a/format file import/File Import Excel/Master Data/data_produk.xlsx
+++ b/format file import/File Import Excel/Master Data/data_produk.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>KETERANGAN INPUT DATA MELALUI EXCEL</t>
   </si>
@@ -124,7 +124,37 @@
     </r>
   </si>
   <si>
-    <t>DISKON</t>
+    <t>HARGA GROSIR #1</t>
+  </si>
+  <si>
+    <t>HARGA GROSIR #2</t>
+  </si>
+  <si>
+    <t>HARGA GROSIR #3</t>
+  </si>
+  <si>
+    <t>JUMLAH MINIMAL GROSIR #1</t>
+  </si>
+  <si>
+    <t>JUMLAH MINIMAL GROSIR #2</t>
+  </si>
+  <si>
+    <t>DISKON GROSIR #1</t>
+  </si>
+  <si>
+    <t>DISKON GROSIR #2</t>
+  </si>
+  <si>
+    <t>JUMLAH MINIMAL GROSIR #3</t>
+  </si>
+  <si>
+    <t>DISKON GROSIR #3</t>
+  </si>
+  <si>
+    <t>HARGA JUAL (RETAIL)</t>
+  </si>
+  <si>
+    <t>DISKON (RETAIL)</t>
   </si>
 </sst>
 </file>
@@ -574,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,14 +617,23 @@
     <col min="3" max="3" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -611,18 +650,45 @@
         <v>16</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>